<commit_message>
BOM updates for revB
</commit_message>
<xml_diff>
--- a/foras-promineo-revB-em/bom/batteryboard.xlsx
+++ b/foras-promineo-revB-em/bom/batteryboard.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Internal Research and Development\RD21 Foras Promineo\KiCad\batteryboard-v01b_SLI_card\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caden\Documents\GitHub\batteryboard\foras-promineo-revB-em\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C60F57-72C8-4E7A-94DB-63AD49AEBCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="batteryboard" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
   <si>
     <t>Item</t>
   </si>
@@ -205,12 +206,54 @@
   </si>
   <si>
     <t>sub PMR100HZPFU10L0</t>
+  </si>
+  <si>
+    <t>TH1</t>
+  </si>
+  <si>
+    <t>MF52C1103F3380</t>
+  </si>
+  <si>
+    <t>Thru-hole</t>
+  </si>
+  <si>
+    <t>NTC</t>
+  </si>
+  <si>
+    <t>presumably pott'd to batteries?</t>
+  </si>
+  <si>
+    <t>TP101,TP102, TP103,TP104</t>
+  </si>
+  <si>
+    <t>wire or keystoone compact TP e.g. p/n 5005</t>
+  </si>
+  <si>
+    <t>J107</t>
+  </si>
+  <si>
+    <t>PCB Testing Connector</t>
+  </si>
+  <si>
+    <t>S2M-110-02-F-D</t>
+  </si>
+  <si>
+    <t>ITD2-10-D</t>
+  </si>
+  <si>
+    <t>Mating Connector Pins</t>
+  </si>
+  <si>
+    <t>Mating Connector Housing</t>
+  </si>
+  <si>
+    <t>T1M82-L-2426-01-L or T1M82-R-2426-01-L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1021,19 +1064,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1378,7 +1421,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>19</v>
       </c>
@@ -1398,7 +1441,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20</v>
       </c>
@@ -1418,7 +1461,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>22</v>
       </c>
@@ -1438,8 +1481,90 @@
         <v>33</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>